<commit_message>
added a period so i can do percentages
</commit_message>
<xml_diff>
--- a/ExcelPython/example.xlsx
+++ b/ExcelPython/example.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -483,7 +483,7 @@
   <sheetData>
     <row r="1" ht="14.4" customHeight="1" s="6">
       <c r="A1" s="7" t="n">
-        <v>42099.56530092589</v>
+        <v>42099.56530092593</v>
       </c>
       <c r="B1" s="8" t="inlineStr">
         <is>
@@ -496,7 +496,7 @@
     </row>
     <row r="2" ht="14.4" customHeight="1" s="6">
       <c r="A2" s="7" t="n">
-        <v>42099.15373842591</v>
+        <v>42099.15373842593</v>
       </c>
       <c r="B2" s="8" t="inlineStr">
         <is>
@@ -509,7 +509,7 @@
     </row>
     <row r="3" ht="14.4" customHeight="1" s="6">
       <c r="A3" s="7" t="n">
-        <v>42100.5325347222</v>
+        <v>42100.53253472222</v>
       </c>
       <c r="B3" s="8" t="inlineStr">
         <is>
@@ -522,7 +522,7 @@
     </row>
     <row r="4" ht="14.4" customHeight="1" s="6">
       <c r="A4" s="7" t="n">
-        <v>42102.37480324071</v>
+        <v>42102.37480324074</v>
       </c>
       <c r="B4" s="8" t="inlineStr">
         <is>
@@ -535,7 +535,7 @@
     </row>
     <row r="5" ht="14.4" customHeight="1" s="6">
       <c r="A5" s="7" t="n">
-        <v>42104.0881944444</v>
+        <v>42104.08819444444</v>
       </c>
       <c r="B5" s="8" t="inlineStr">
         <is>
@@ -548,7 +548,7 @@
     </row>
     <row r="6" ht="14.4" customHeight="1" s="6">
       <c r="A6" s="7" t="n">
-        <v>42104.7573726852</v>
+        <v>42104.75737268518</v>
       </c>
       <c r="B6" s="8" t="inlineStr">
         <is>
@@ -561,7 +561,7 @@
     </row>
     <row r="7" ht="14.4" customHeight="1" s="6">
       <c r="A7" s="7" t="n">
-        <v>42104.11164351851</v>
+        <v>42104.11164351852</v>
       </c>
       <c r="B7" s="8" t="inlineStr">
         <is>
@@ -585,14 +585,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="B1:B1"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="0" outlineLevelRow="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Cat</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>